<commit_message>
Model data bases with 4 in and outputs
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/diesel/Model_Data_Base_diesel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/diesel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/luc_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/diesel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="280" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E7325245-4B28-4D9D-A364-5F836528474E}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="13_ncr:1_{F150E804-DDA9-4EB4-B6B4-76CF44ACC28F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD7F9579-AA48-4111-8FCD-B7C7EC2A82CE}"/>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="-19815" windowWidth="24285" windowHeight="13740" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{50334894-9481-4F8E-BD29-206032E10C62}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -504,10 +504,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,7 +914,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{576C757C-091A-46DF-949E-B17661031FDE}">
   <dimension ref="A1:AJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight"/>
     </sheetView>
@@ -1288,7 +1284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C870BDA0-9E4C-481D-87BE-9D47789809C8}">
   <dimension ref="A1:AA5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="V1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1588,7 +1584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{981CFA5E-60F3-446F-A856-2FA65B76879A}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>